<commit_message>
Changes:1.) Invoice - Updated.
</commit_message>
<xml_diff>
--- a/etc/invoice-templates/Den-Internet-Bill.xlsx
+++ b/etc/invoice-templates/Den-Internet-Bill.xlsx
@@ -1992,7 +1992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -3909,8 +3909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>